<commit_message>
update test case ids for store pets
</commit_message>
<xml_diff>
--- a/StoreData.xlsx
+++ b/StoreData.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,7 +382,7 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -647,7 +647,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +659,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>